<commit_message>
added lots of changes for journal
</commit_message>
<xml_diff>
--- a/params.xlsx
+++ b/params.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sebas\Documents\MATLAB\ProCiencia\Journal2024\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{601B9525-AEA4-48CA-847A-C0DAABF542A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F13969E-3D4E-4709-BE5B-B68E53568AE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -517,7 +517,7 @@
   <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L9" sqref="L9"/>
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
@@ -660,16 +660,16 @@
         <v>25</v>
       </c>
       <c r="H4" s="17">
-        <v>1</v>
+        <v>1.03</v>
       </c>
       <c r="I4" s="17">
-        <v>2.6</v>
+        <v>2.63</v>
       </c>
       <c r="J4" s="17">
-        <v>0.45</v>
+        <v>0.49</v>
       </c>
       <c r="K4" s="17">
-        <v>2.2000000000000002</v>
+        <v>2.14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>